<commit_message>
CHARMS RAS changed tags to @RAS_Regression tags
</commit_message>
<xml_diff>
--- a/src/test/java/ServiceNow/CHARMS/Resources/RASScenario_Consent_Age_14-17.xlsx
+++ b/src/test/java/ServiceNow/CHARMS/Resources/RASScenario_Consent_Age_14-17.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juarezds/Desktop/CBIIT-Test-Automation/src/test/java/ServiceNow/CHARMS/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muzipovay2/AquaProjects/CBIIT-Test-Automation/src/test/java/ServiceNow/CHARMS/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859C3572-B6AE-CD4C-B935-69D2B68B78C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D99894-5656-2140-820D-566F1803A647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7240" yWindow="920" windowWidth="22940" windowHeight="14300" xr2:uid="{54739BCC-024D-1B43-9BD3-233381306DEA}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" xr2:uid="{54739BCC-024D-1B43-9BD3-233381306DEA}"/>
   </bookViews>
   <sheets>
-    <sheet name="screenerScenario1" sheetId="1" r:id="rId1"/>
+    <sheet name="screenerScenarioAge14-17" sheetId="1" r:id="rId1"/>
     <sheet name="IIQScenario1" sheetId="2" r:id="rId2"/>
     <sheet name="RASSurveyScenario1" sheetId="7" r:id="rId3"/>
   </sheets>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="347">
   <si>
     <t>Question</t>
   </si>
@@ -52,28 +52,10 @@
     <t>I am completing this form for myself</t>
   </si>
   <si>
-    <t>Middle Initial</t>
-  </si>
-  <si>
     <t>T</t>
   </si>
   <si>
-    <t>First name</t>
-  </si>
-  <si>
-    <t>Last name</t>
-  </si>
-  <si>
     <t>What is your date of birth?</t>
-  </si>
-  <si>
-    <t>Date of birth month</t>
-  </si>
-  <si>
-    <t>April</t>
-  </si>
-  <si>
-    <t>Date of birth year</t>
   </si>
   <si>
     <t>What was your sex assigned at birth?</t>
@@ -1110,24 +1092,76 @@
     <t>Do you have any of the following issues with your ears?  Please select all that apply. Option 4</t>
   </si>
   <si>
-    <t>charmsras1@yahoo.com</t>
-  </si>
-  <si>
-    <t>April 1, 1990</t>
-  </si>
-  <si>
-    <t>DiegoFirstTest</t>
-  </si>
-  <si>
-    <t>JuarezTest</t>
+    <t>I am completing this form for someone else</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>CHARMS RAS Parent</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>What is the name of the person who may be eligible for this study? First</t>
+  </si>
+  <si>
+    <t>What is the name of the person who may be eligible for this study? MI</t>
+  </si>
+  <si>
+    <t>CHARMS RAS Minor</t>
+  </si>
+  <si>
+    <t>What is the name of the person who may be eligible for this study? Last</t>
+  </si>
+  <si>
+    <t>What is your name?</t>
+  </si>
+  <si>
+    <t>First name</t>
+  </si>
+  <si>
+    <t>Middle Initial</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
+  <si>
+    <t>What is the name of the person who may be eligible for this study?</t>
+  </si>
+  <si>
+    <t>CHARMS RAS Minor Test</t>
+  </si>
+  <si>
+    <t>What is your relationship to the participant?</t>
+  </si>
+  <si>
+    <t>Are you the legal guardian of the participant?</t>
+  </si>
+  <si>
+    <t>The next set of questions will collect basic information about the participant.</t>
+  </si>
+  <si>
+    <t>Date of birth of the participant.</t>
+  </si>
+  <si>
+    <t>Is the participant alive?</t>
+  </si>
+  <si>
+    <t>CHARMS RAS Parent Test</t>
+  </si>
+  <si>
+    <t>consent_participant@yopmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -1228,7 +1262,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1547,10 +1581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AAA49E6-03DB-BC47-B34D-065780B05137}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1572,282 +1606,335 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>338</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>330</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>5</v>
+        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>331</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>335</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="15" t="s">
         <v>333</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>334</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>10</v>
+        <v>345</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="4">
-        <v>1990</v>
+        <v>335</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>336</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>337</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>15</v>
+        <v>327</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>340</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>329</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>20</v>
+        <v>342</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>21</v>
+        <v>343</v>
+      </c>
+      <c r="B14" s="15">
+        <v>40116</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="4">
-        <v>22015</v>
+        <v>344</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>332</v>
+        <v>10</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>40</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="4">
+        <v>22015</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>41</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="323" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>266</v>
+      <c r="B42" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="323" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B18" r:id="rId1" xr:uid="{F82FA76E-2358-814A-8E85-BCB9636B476E}"/>
-    <hyperlink ref="B19" r:id="rId2" xr:uid="{9CF4B7EF-6998-144B-B594-2EFE15A9CFC2}"/>
+    <hyperlink ref="B25" r:id="rId1" xr:uid="{F82FA76E-2358-814A-8E85-BCB9636B476E}"/>
+    <hyperlink ref="B26" r:id="rId2" xr:uid="{9CF4B7EF-6998-144B-B594-2EFE15A9CFC2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1878,31 +1965,31 @@
     </row>
     <row r="2" spans="1:2" ht="170" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="272" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>3</v>
@@ -1910,71 +1997,71 @@
     </row>
     <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B14" s="4">
         <v>10</v>
@@ -1982,7 +2069,7 @@
     </row>
     <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B15" s="4">
         <v>2004</v>
@@ -1990,7 +2077,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B16" s="6">
         <v>38301</v>
@@ -1998,143 +2085,143 @@
     </row>
     <row r="17" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B34" s="4">
         <v>4.5</v>
@@ -2142,15 +2229,15 @@
     </row>
     <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B36" s="4">
         <v>19</v>
@@ -2158,7 +2245,7 @@
     </row>
     <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B37" s="4">
         <v>34</v>
@@ -2166,47 +2253,47 @@
     </row>
     <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B43" s="4">
         <v>70</v>
@@ -2214,15 +2301,15 @@
     </row>
     <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B45" s="4">
         <v>128</v>
@@ -2230,7 +2317,7 @@
     </row>
     <row r="46" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="B46" s="4">
         <v>130</v>
@@ -2238,7 +2325,7 @@
     </row>
     <row r="47" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B47" s="4">
         <v>129</v>
@@ -2246,7 +2333,7 @@
     </row>
     <row r="48" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="B48" s="4">
         <v>100</v>
@@ -2254,7 +2341,7 @@
     </row>
     <row r="49" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="B49" s="4">
         <v>101</v>
@@ -2262,82 +2349,82 @@
     </row>
     <row r="50" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="102" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="102" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="136" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2370,31 +2457,31 @@
     </row>
     <row r="2" spans="1:2" ht="372" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="136" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>3</v>
@@ -2402,39 +2489,39 @@
     </row>
     <row r="6" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B10" s="10">
         <v>45</v>
@@ -2442,23 +2529,23 @@
     </row>
     <row r="11" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B13" s="10">
         <v>53</v>
@@ -2466,103 +2553,103 @@
     </row>
     <row r="14" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B26" s="10">
         <v>108</v>
@@ -2570,7 +2657,7 @@
     </row>
     <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B27" s="10">
         <v>600</v>
@@ -2578,300 +2665,300 @@
     </row>
     <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="12" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="12" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="12" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="12" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="12" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="12" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="12" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="12" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A56" s="12" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="12" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="12" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="13" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A60" s="12" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="13" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" s="12" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A63" s="12" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="13" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="13" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B65" s="10">
         <v>1</v>
@@ -2879,786 +2966,786 @@
     </row>
     <row r="66" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="13" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="13" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="13" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="13" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="13" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="13" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="13" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="13" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="13" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="13" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="13" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="13" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="13" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="13" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="13" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="13" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="13" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="13" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="13" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="13" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="13" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="13" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="13" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="13" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="13" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="13" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="13" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="13" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="13" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B94" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="13" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="13" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="13" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="13" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B98" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A99" s="12" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="12" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="13" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B101" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="13" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B102" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="13" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B103" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="13" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B104" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="13" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B105" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="13" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B106" s="10" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="13" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B107" s="10" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="13" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B108" s="10" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="13" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B109" s="10" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="13" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B110" s="10" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="13" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B111" s="10" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="13" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B112" s="10" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="13" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B113" s="10" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="13" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B114" s="10" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="13" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B115" s="10" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="13" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B116" s="10" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="13" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B117" s="10" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="13" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B118" s="10" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="13" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B119" s="10" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="13" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B120" s="10" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A121" s="12" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B121" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="13" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B122" s="10" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="13" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B123" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A124" s="12" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="B124" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="13" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B125" s="10" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="13" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="B126" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="13" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B127" s="10" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="13" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B128" s="10" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="13" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B129" s="10" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="13" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="B130" s="10" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A131" s="13" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="B131" s="10" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A132" s="13" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="B132" s="10" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A133" s="12" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="B133" s="11" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" s="12" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="B134" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="13" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="B135" s="10" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A136" s="13" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B136" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" s="12" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="B137" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A138" s="12" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B138" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="12" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B139" s="10" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" s="12" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="B140" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" s="12" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B141" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A142" s="12" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="B142" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A143" s="12" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B143" s="10" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="12" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B144" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A145" s="12" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B145" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A146" s="12" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="B146" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A147" s="12" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B147" s="11" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A148" s="12" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="B148" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" s="12" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="B149" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A150" s="12" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="B150" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" s="12" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="B151" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A152" s="12" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="B152" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A153" s="12" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="B153" s="10" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" s="12" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B154" s="10" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A155" s="12" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B155" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A156" s="12" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="B156" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A157" s="12" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="B157" s="10" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A158" s="12" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="B158" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A159" s="12" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="B159" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A160" s="12" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B160" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A161" s="12" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="B161" s="10" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A162" s="12" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="B162" s="10" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="128" x14ac:dyDescent="0.2">
       <c r="A163" s="12" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="B163" s="11" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>